<commit_message>
Created the skeleton of the PySide2 app.
</commit_message>
<xml_diff>
--- a/2 User Database.xlsx
+++ b/2 User Database.xlsx
@@ -1,89 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tandapay\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5469BC0A-8C9F-4E6C-B29A-794C45C661D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2 User Database" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2 User Database" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>UsRec1</t>
-  </si>
-  <si>
-    <t>UsRec2</t>
-  </si>
-  <si>
-    <t>UsRec3</t>
-  </si>
-  <si>
-    <t>UsRec4</t>
-  </si>
-  <si>
-    <t>UsRec5</t>
-  </si>
-  <si>
-    <t>UsRec6</t>
-  </si>
-  <si>
-    <t>UsRec7</t>
-  </si>
-  <si>
-    <t>UsRec8</t>
-  </si>
-  <si>
-    <t>UsRec9</t>
-  </si>
-  <si>
-    <t>UsRec10</t>
-  </si>
-  <si>
-    <t>UsRec11</t>
-  </si>
-  <si>
-    <t>UsRec12</t>
-  </si>
-  <si>
-    <t>UsRec13</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,22 +53,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,84 +427,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>UsRec1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UsRec2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>UsRec3</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>UsRec4</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>UsRec5</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>UsRec6</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>UsRec7</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>UsRec8</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>UsRec9</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>UsRec10</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>UsRec11</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>UsRec12</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>UsRec13</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+    </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>